<commit_message>
Fixed some star loctions and magnitudes
</commit_message>
<xml_diff>
--- a/starMap.xlsx
+++ b/starMap.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leif/Documents/sinkt/SourceCode/Python/Space_and_Astronomy/NEA_Tracking_Calcs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{096C252A-60AD-624B-BEEA-961E792068A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB420782-E3AC-054B-8392-BF8FC0945599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4460" yWindow="3660" windowWidth="28400" windowHeight="17260" xr2:uid="{3419C8CB-29DD-3746-BD00-8C3618883330}"/>
   </bookViews>
   <sheets>
     <sheet name="starData" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -144,9 +144,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="0.0000"/>
-    <numFmt numFmtId="171" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="172" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;????_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;????_);_(@_)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -185,32 +185,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1280,7 +1279,7 @@
                   <c:v>0.2305763888888889</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.2305763888888889</c:v>
+                  <c:v>0.22534722222222223</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.25167129629629631</c:v>
@@ -1331,7 +1330,7 @@
                   <c:v>-0.29833333333333334</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-0.29833333333333334</c:v>
+                  <c:v>-2.3963888888888887</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>9.6474722222222216</c:v>
@@ -3874,12 +3873,11 @@
   <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="10.83203125" style="2"/>
     <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -3894,16 +3892,16 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>11</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -3912,13 +3910,13 @@
       <c r="I1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -3932,38 +3930,38 @@
       <c r="C2" s="1">
         <v>5</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>0.21844560185185183</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <f>-(8+12/60+2.9/3600)</f>
         <v>-8.2008055555555543</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2" s="5">
         <v>0.15</v>
       </c>
-      <c r="H2" s="8" cm="1">
+      <c r="H2" s="7" cm="1">
         <f t="array" ref="H2">SUMPRODUCT(60^{0,-1,-2},{217,39,39})</f>
         <v>217.66083333333333</v>
       </c>
-      <c r="I2" s="8" cm="1">
+      <c r="I2" s="7" cm="1">
         <f t="array" ref="I2">SUMPRODUCT(60^{0,-1,-2},{31,52,9.8})</f>
         <v>31.869388888888889</v>
       </c>
-      <c r="J2" s="9">
+      <c r="J2" s="8">
         <f>E2*24*15</f>
         <v>78.640416666666667</v>
       </c>
-      <c r="K2" s="11">
+      <c r="K2" s="10">
         <f>-(J2-AVERAGE($J$2:$J$15))</f>
-        <v>4.4046845238095358</v>
-      </c>
-      <c r="L2" s="12">
+        <v>4.2702202380952343</v>
+      </c>
+      <c r="L2" s="11">
         <f>F2-AVERAGE($F$2:$F$15)</f>
-        <v>-9.4281706349206331</v>
+        <v>-9.2783095238095221</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
@@ -3976,38 +3974,38 @@
       <c r="C3" s="1">
         <v>5</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>0.21379976851851853</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <f>-(5+5/60+9.6/3600)</f>
         <v>-5.0859999999999994</v>
       </c>
-      <c r="G3" s="6">
-        <v>0.15</v>
-      </c>
-      <c r="H3" s="8" cm="1">
+      <c r="G3" s="5">
+        <v>2.75</v>
+      </c>
+      <c r="H3" s="7" cm="1">
         <f t="array" ref="H3">SUMPRODUCT(60^{0,-1,-2},{221,9,4})</f>
         <v>221.15111111111111</v>
       </c>
-      <c r="I3" s="8" cm="1">
+      <c r="I3" s="7" cm="1">
         <f t="array" ref="I3">SUMPRODUCT(60^{0,-1,-2},{33,50,8.9})</f>
         <v>33.835805555555559</v>
       </c>
-      <c r="J3" s="9">
+      <c r="J3" s="8">
         <f t="shared" ref="J3:J15" si="0">E3*24*15</f>
         <v>76.967916666666667</v>
       </c>
-      <c r="K3" s="11">
+      <c r="K3" s="10">
         <f t="shared" ref="K3:K15" si="1">-(J3-AVERAGE($J$2:$J$15))</f>
-        <v>6.0771845238095352</v>
-      </c>
-      <c r="L3" s="12">
+        <v>5.9427202380952338</v>
+      </c>
+      <c r="L3" s="11">
         <f t="shared" ref="L3:L15" si="2">F3-AVERAGE($F$2:$F$15)</f>
-        <v>-6.3133650793650791</v>
+        <v>-6.1635039682539681</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
@@ -4020,38 +4018,38 @@
       <c r="C4" s="1">
         <v>5</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>0.23374074074074072</v>
       </c>
-      <c r="F4" s="5" cm="1">
+      <c r="F4" s="4" cm="1">
         <f t="array" ref="F4">-SUMPRODUCT(60^{0,-1,-2},{5,54,50.9})</f>
         <v>-5.9141388888888891</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="5">
         <v>2.5</v>
       </c>
-      <c r="H4" s="8" cm="1">
+      <c r="H4" s="7" cm="1">
         <f t="array" ref="H4">SUMPRODUCT(60^{0,-1,-2},{213,12,34.6})</f>
         <v>213.20961111111109</v>
       </c>
-      <c r="I4" s="8" cm="1">
+      <c r="I4" s="7" cm="1">
         <f t="array" ref="I4">SUMPRODUCT(60^{0,-1,-2},{36,9,40})</f>
         <v>36.161111111111111</v>
       </c>
-      <c r="J4" s="9">
+      <c r="J4" s="8">
         <f t="shared" si="0"/>
         <v>84.146666666666661</v>
       </c>
-      <c r="K4" s="11">
+      <c r="K4" s="10">
         <f t="shared" si="1"/>
-        <v>-1.1015654761904585</v>
-      </c>
-      <c r="L4" s="12">
+        <v>-1.23602976190476</v>
+      </c>
+      <c r="L4" s="11">
         <f t="shared" si="2"/>
-        <v>-7.1415039682539678</v>
+        <v>-6.9916428571428577</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -4064,38 +4062,38 @@
       <c r="C5" s="1">
         <v>5</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>0.24151620370370372</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <f>-(9+40/60+7.1/3600)</f>
         <v>-9.6686388888888875</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="5">
         <v>2.0499999999999998</v>
       </c>
-      <c r="H5" s="8" cm="1">
+      <c r="H5" s="7" cm="1">
         <f t="array" ref="H5">SUMPRODUCT(60^{0,-1,-2},{208,1,3.5})</f>
         <v>208.01763888888891</v>
       </c>
-      <c r="I5" s="8" cm="1">
+      <c r="I5" s="7" cm="1">
         <f t="array" ref="I5">SUMPRODUCT(60^{0,-1,-2},{33,50,28})</f>
         <v>33.841111111111111</v>
       </c>
-      <c r="J5" s="9">
+      <c r="J5" s="8">
         <f t="shared" si="0"/>
         <v>86.94583333333334</v>
       </c>
-      <c r="K5" s="11">
+      <c r="K5" s="10">
         <f t="shared" si="1"/>
-        <v>-3.9007321428571373</v>
-      </c>
-      <c r="L5" s="12">
+        <v>-4.0351964285714388</v>
+      </c>
+      <c r="L5" s="11">
         <f t="shared" si="2"/>
-        <v>-10.896003968253966</v>
+        <v>-10.746142857142855</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
@@ -4108,38 +4106,38 @@
       <c r="C6" s="1">
         <v>5</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>0.23666666666666666</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <f>-(1+56/60+30.4/3600)</f>
         <v>-1.9417777777777778</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>1.85</v>
       </c>
-      <c r="H6" s="8" cm="1">
+      <c r="H6" s="7" cm="1">
         <f t="array" ref="H6">SUMPRODUCT(60^{0,-1,-2},{213,42,47.9})</f>
         <v>213.71330555555554</v>
       </c>
-      <c r="I6" s="8" cm="1">
+      <c r="I6" s="7" cm="1">
         <f t="array" ref="I6">SUMPRODUCT(60^{0,-1,-2},{40,20,0.7})</f>
         <v>40.333527777777782</v>
       </c>
-      <c r="J6" s="9">
+      <c r="J6" s="8">
         <f t="shared" si="0"/>
         <v>85.199999999999989</v>
       </c>
-      <c r="K6" s="11">
+      <c r="K6" s="10">
         <f t="shared" si="1"/>
-        <v>-2.154898809523786</v>
-      </c>
-      <c r="L6" s="12">
+        <v>-2.2893630952380875</v>
+      </c>
+      <c r="L6" s="11">
         <f t="shared" si="2"/>
-        <v>-3.169142857142857</v>
+        <v>-3.019281746031746</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
@@ -4152,38 +4150,38 @@
       <c r="C7" s="1">
         <v>5</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>0.23349768518518518</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <f>-(1+12/60+4.2/3600)</f>
         <v>-1.2011666666666667</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>1.65</v>
       </c>
-      <c r="H7" s="8" cm="1">
+      <c r="H7" s="7" cm="1">
         <f t="array" ref="H7">SUMPRODUCT(60^{0,-1,-2},{215,28,32.6})</f>
         <v>215.47572222222223</v>
       </c>
-      <c r="I7" s="8" cm="1">
+      <c r="I7" s="7" cm="1">
         <f t="array" ref="I7">SUMPRODUCT(60^{0,-1,-2},{40,31,53})</f>
         <v>40.531388888888891</v>
       </c>
-      <c r="J7" s="9">
+      <c r="J7" s="8">
         <f t="shared" si="0"/>
         <v>84.05916666666667</v>
       </c>
-      <c r="K7" s="11">
+      <c r="K7" s="10">
         <f t="shared" si="1"/>
-        <v>-1.0140654761904671</v>
-      </c>
-      <c r="L7" s="12">
+        <v>-1.1485297619047685</v>
+      </c>
+      <c r="L7" s="11">
         <f t="shared" si="2"/>
-        <v>-2.4285317460317462</v>
+        <v>-2.2786706349206352</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -4196,38 +4194,38 @@
       <c r="C8" s="1">
         <v>5</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>0.2305763888888889</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <f>-(0+17/60+54/3600)</f>
         <v>-0.29833333333333334</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>2.4</v>
       </c>
-      <c r="H8" s="8" cm="1">
+      <c r="H8" s="7" cm="1">
         <f t="array" ref="H8">SUMPRODUCT(60^{0,-1,-2},{217,14,37.7})</f>
         <v>217.24380555555555</v>
       </c>
-      <c r="I8" s="8" cm="1">
+      <c r="I8" s="7" cm="1">
         <f t="array" ref="I8">SUMPRODUCT(60^{0,-1,-2},{40,53,4.4})</f>
         <v>40.884555555555558</v>
       </c>
-      <c r="J8" s="9">
+      <c r="J8" s="8">
         <f t="shared" si="0"/>
         <v>83.007500000000007</v>
       </c>
-      <c r="K8" s="11">
+      <c r="K8" s="10">
         <f t="shared" si="1"/>
-        <v>3.7601190476195256E-2</v>
-      </c>
-      <c r="L8" s="12">
+        <v>-9.6863095238106212E-2</v>
+      </c>
+      <c r="L8" s="11">
         <f t="shared" si="2"/>
-        <v>-1.5256984126984126</v>
+        <v>-1.3758373015873018</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -4240,38 +4238,38 @@
       <c r="C9" s="1">
         <v>5</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="4">
-        <v>0.2305763888888889</v>
-      </c>
-      <c r="F9" s="5">
-        <f>-(0+17/60+54/3600)</f>
-        <v>-0.29833333333333334</v>
-      </c>
-      <c r="G9" s="6">
+      <c r="E9" s="3">
+        <v>0.22534722222222223</v>
+      </c>
+      <c r="F9" s="4" cm="1">
+        <f t="array" ref="F9">-SUMPRODUCT(60^{0,-1,-2},{2,23,47})</f>
+        <v>-2.3963888888888887</v>
+      </c>
+      <c r="G9" s="5">
         <v>3.35</v>
       </c>
-      <c r="H9" s="8" cm="1">
+      <c r="H9" s="7" cm="1">
         <f t="array" ref="H9">SUMPRODUCT(60^{0,-1,-2},{218,11,34.2})</f>
         <v>218.19283333333334</v>
       </c>
-      <c r="I9" s="8" cm="1">
+      <c r="I9" s="7" cm="1">
         <f t="array" ref="I9">SUMPRODUCT(60^{0,-1,-2},{38,9,48.6})</f>
         <v>38.163499999999999</v>
       </c>
-      <c r="J9" s="9">
+      <c r="J9" s="8">
         <f t="shared" si="0"/>
-        <v>83.007500000000007</v>
-      </c>
-      <c r="K9" s="11">
+        <v>81.125</v>
+      </c>
+      <c r="K9" s="10">
         <f t="shared" si="1"/>
-        <v>3.7601190476195256E-2</v>
-      </c>
-      <c r="L9" s="12">
+        <v>1.7856369047619012</v>
+      </c>
+      <c r="L9" s="11">
         <f t="shared" si="2"/>
-        <v>-1.5256984126984126</v>
+        <v>-3.4738928571428573</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -4284,38 +4282,38 @@
       <c r="C10" s="1">
         <v>5</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" t="s">
         <v>18</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>0.25167129629629631</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <f>+(9+38/60+50.9/3600)</f>
         <v>9.6474722222222216</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <v>4.3</v>
       </c>
-      <c r="H10" s="8" cm="1">
+      <c r="H10" s="7" cm="1">
         <f t="array" ref="H10">SUMPRODUCT(60^{0,-1,-2},{213,27,16.4})</f>
         <v>213.45455555555554</v>
       </c>
-      <c r="I10" s="8" cm="1">
+      <c r="I10" s="7" cm="1">
         <f t="array" ref="I10">SUMPRODUCT(60^{0,-1,-2},{53,6,41})</f>
         <v>53.111388888888889</v>
       </c>
-      <c r="J10" s="9">
+      <c r="J10" s="8">
         <f t="shared" si="0"/>
         <v>90.601666666666659</v>
       </c>
-      <c r="K10" s="11">
+      <c r="K10" s="10">
         <f t="shared" si="1"/>
-        <v>-7.5565654761904568</v>
-      </c>
-      <c r="L10" s="12">
+        <v>-7.6910297619047583</v>
+      </c>
+      <c r="L10" s="11">
         <f t="shared" si="2"/>
-        <v>8.4201071428571428</v>
+        <v>8.5699682539682538</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -4328,38 +4326,38 @@
       <c r="C11" s="1">
         <v>5</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D11" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>0.24666319444444443</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <f>+(7+24/60+27.6/3600)</f>
         <v>7.4076666666666666</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <v>0.45</v>
       </c>
-      <c r="H11" s="8" cm="1">
+      <c r="H11" s="7" cm="1">
         <f t="array" ref="H11">SUMPRODUCT(60^{0,-1,-2},{214,33,58})</f>
         <v>214.56611111111113</v>
       </c>
-      <c r="I11" s="8" cm="1">
+      <c r="I11" s="7" cm="1">
         <f t="array" ref="I11">SUMPRODUCT(60^{0,-1,-2},{50,19,58})</f>
         <v>50.332777777777778</v>
       </c>
-      <c r="J11" s="9">
+      <c r="J11" s="8">
         <f t="shared" si="0"/>
         <v>88.798749999999998</v>
       </c>
-      <c r="K11" s="11">
+      <c r="K11" s="10">
         <f t="shared" si="1"/>
-        <v>-5.7536488095237956</v>
-      </c>
-      <c r="L11" s="12">
+        <v>-5.8881130952380971</v>
+      </c>
+      <c r="L11" s="11">
         <f t="shared" si="2"/>
-        <v>6.180301587301587</v>
+        <v>6.330162698412698</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -4372,38 +4370,38 @@
       <c r="C12" s="1">
         <v>5</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" t="s">
         <v>5</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>0.22580092592592593</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <f>+(6+21/60+0.9/3600)</f>
         <v>6.35025</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="5">
         <v>1.6</v>
       </c>
-      <c r="H12" s="8" cm="1">
+      <c r="H12" s="7" cm="1">
         <f t="array" ref="H12">SUMPRODUCT(60^{0,-1,-2},{223,42,12})</f>
         <v>223.70333333333332</v>
       </c>
-      <c r="I12" s="8" cm="1">
+      <c r="I12" s="7" cm="1">
         <f t="array" ref="I12">SUMPRODUCT(60^{0,-1,-2},{45,54,8})</f>
         <v>45.902222222222221</v>
       </c>
-      <c r="J12" s="9">
+      <c r="J12" s="8">
         <f t="shared" si="0"/>
         <v>81.288333333333341</v>
       </c>
-      <c r="K12" s="11">
+      <c r="K12" s="10">
         <f t="shared" si="1"/>
-        <v>1.7567678571428615</v>
-      </c>
-      <c r="L12" s="12">
+        <v>1.6223035714285601</v>
+      </c>
+      <c r="L12" s="11">
         <f t="shared" si="2"/>
-        <v>5.1228849206349203</v>
+        <v>5.2727460317460313</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -4416,38 +4414,38 @@
       <c r="C13" s="1">
         <v>5</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>0.20129629629629631</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <f>+(6+57/60+43.6/3600)</f>
         <v>6.9621111111111116</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="5">
         <v>1.6</v>
       </c>
-      <c r="H13" s="8" cm="1">
+      <c r="H13" s="7" cm="1">
         <f t="array" ref="H13">SUMPRODUCT(60^{0,-1,-2},{234,13,50})</f>
         <v>234.23055555555555</v>
       </c>
-      <c r="I13" s="8" cm="1">
+      <c r="I13" s="7" cm="1">
         <f t="array" ref="I13">SUMPRODUCT(60^{0,-1,-2},{41,30,2})</f>
         <v>41.500555555555557</v>
       </c>
-      <c r="J13" s="9">
+      <c r="J13" s="8">
         <f t="shared" si="0"/>
         <v>72.466666666666669</v>
       </c>
-      <c r="K13" s="11">
+      <c r="K13" s="10">
         <f t="shared" si="1"/>
-        <v>10.578434523809534</v>
-      </c>
-      <c r="L13" s="12">
+        <v>10.443970238095233</v>
+      </c>
+      <c r="L13" s="11">
         <f t="shared" si="2"/>
-        <v>5.7347460317460328</v>
+        <v>5.8846071428571429</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -4460,38 +4458,38 @@
       <c r="C14" s="1">
         <v>5</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>0.23253009259259261</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <f>+(9+29/60+24.4/3600)</f>
         <v>9.4901111111111103</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="5">
         <v>4.3499999999999996</v>
       </c>
-      <c r="H14" s="8" cm="1">
+      <c r="H14" s="7" cm="1">
         <f t="array" ref="H14">SUMPRODUCT(60^{0,-1,-2},{223,1,15})</f>
         <v>223.02083333333334</v>
       </c>
-      <c r="I14" s="8" cm="1">
+      <c r="I14" s="7" cm="1">
         <f t="array" ref="I14">SUMPRODUCT(60^{0,-1,-2},{49,49,37})</f>
         <v>49.82694444444445</v>
       </c>
-      <c r="J14" s="9">
+      <c r="J14" s="8">
         <f t="shared" si="0"/>
         <v>83.710833333333341</v>
       </c>
-      <c r="K14" s="11">
+      <c r="K14" s="10">
         <f t="shared" si="1"/>
-        <v>-0.66573214285713789</v>
-      </c>
-      <c r="L14" s="12">
+        <v>-0.80019642857143936</v>
+      </c>
+      <c r="L14" s="11">
         <f t="shared" si="2"/>
-        <v>8.2627460317460315</v>
+        <v>8.4126071428571425</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -4504,54 +4502,50 @@
       <c r="C15" s="1">
         <v>5</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" t="s">
         <v>4</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>0.23275046296296295</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <f>+(9+56/60+4.9/3600)</f>
         <v>9.9346944444444443</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="5">
         <v>3.5</v>
       </c>
-      <c r="H15" s="8" cm="1">
+      <c r="H15" s="7" cm="1">
         <f t="array" ref="H15">SUMPRODUCT(60^{0,-1,-2},{223,16,12})</f>
         <v>223.27</v>
       </c>
-      <c r="I15" s="8" cm="1">
+      <c r="I15" s="7" cm="1">
         <f t="array" ref="I15">SUMPRODUCT(60^{0,-1,-2},{50,14,57})</f>
         <v>50.249166666666667</v>
       </c>
-      <c r="J15" s="9">
+      <c r="J15" s="8">
         <f t="shared" si="0"/>
         <v>83.790166666666664</v>
       </c>
-      <c r="K15" s="11">
+      <c r="K15" s="10">
         <f t="shared" si="1"/>
-        <v>-0.7450654761904616</v>
-      </c>
-      <c r="L15" s="12">
+        <v>-0.87952976190476306</v>
+      </c>
+      <c r="L15" s="11">
         <f t="shared" si="2"/>
-        <v>8.7073293650793655</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D16" s="2"/>
-      <c r="E16"/>
+        <v>8.8571904761904765</v>
+      </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="J17" s="10"/>
+      <c r="J17" s="9"/>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.2">
-      <c r="B26" s="7"/>
-      <c r="D26" s="7"/>
+      <c r="B26" s="6"/>
+      <c r="D26" s="6"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" s="7"/>
-      <c r="D34" s="7"/>
+      <c r="B34" s="6"/>
+      <c r="D34" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>